<commit_message>
Version 2.0 more friendly to users
</commit_message>
<xml_diff>
--- a/outp.xlsx
+++ b/outp.xlsx
@@ -734,9 +734,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
@@ -1050,7 +1047,7 @@
       <c r="A12" s="2">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1058,10 +1055,10 @@
       <c r="A13" s="2">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1132,10 +1129,10 @@
       <c r="A14" s="2">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>48</v>
       </c>
       <c r="Q14" s="1" t="s">
@@ -1164,10 +1161,10 @@
       <c r="A15" s="2">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
       <c r="Q15" s="1" t="s">
@@ -1196,10 +1193,10 @@
       <c r="A16" s="2">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>40</v>
       </c>
       <c r="Q16" s="1" t="s">
@@ -1219,10 +1216,10 @@
       <c r="A17" s="2">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>49</v>
       </c>
       <c r="Q17" s="1" t="s">
@@ -1242,10 +1239,10 @@
       <c r="A18" s="2">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1304,10 +1301,10 @@
       <c r="A19" s="2">
         <v>7</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1366,10 +1363,10 @@
       <c r="A20" s="2">
         <v>8</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1398,10 +1395,10 @@
       <c r="A21" s="2">
         <v>9</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1430,7 +1427,7 @@
       <c r="A22" s="2">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1438,10 +1435,10 @@
       <c r="A23" s="2">
         <v>11</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1512,10 +1509,10 @@
       <c r="A24" s="2">
         <v>12</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1541,10 +1538,10 @@
       <c r="A25" s="2">
         <v>13</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1570,10 +1567,10 @@
       <c r="A26" s="2">
         <v>14</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>50</v>
       </c>
       <c r="M26" s="1" t="s">
@@ -1590,10 +1587,10 @@
       <c r="A27" s="2">
         <v>15</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>51</v>
       </c>
       <c r="M27" s="1" t="s">
@@ -1610,10 +1607,10 @@
       <c r="A28" s="2">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1627,10 +1624,10 @@
       <c r="A29" s="2">
         <v>17</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1644,7 +1641,7 @@
       <c r="A30" s="2">
         <v>18</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1652,10 +1649,10 @@
       <c r="A31" s="2">
         <v>19</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1726,10 +1723,10 @@
       <c r="A32" s="2">
         <v>20</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>48</v>
       </c>
       <c r="Q32" s="1" t="s">
@@ -1752,10 +1749,10 @@
       <c r="A33" s="2">
         <v>21</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>39</v>
       </c>
       <c r="Q33" s="1" t="s">
@@ -1778,10 +1775,10 @@
       <c r="A34" s="2">
         <v>22</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1834,10 +1831,10 @@
       <c r="A35" s="2">
         <v>23</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1890,10 +1887,10 @@
       <c r="A36" s="2">
         <v>24</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1952,10 +1949,10 @@
       <c r="A37" s="2">
         <v>25</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -2014,7 +2011,7 @@
       <c r="A38" s="2">
         <v>26</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2022,10 +2019,10 @@
       <c r="A39" s="2">
         <v>27</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2096,10 +2093,10 @@
       <c r="A40" s="2">
         <v>28</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>48</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -2110,10 +2107,10 @@
       <c r="A41" s="2">
         <v>29</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>39</v>
       </c>
       <c r="R41" s="1" t="s">
@@ -2124,10 +2121,10 @@
       <c r="A42" s="2">
         <v>30</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>40</v>
       </c>
       <c r="Q42" s="1" t="s">
@@ -2153,10 +2150,10 @@
       <c r="A43" s="2">
         <v>31</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>49</v>
       </c>
       <c r="Q43" s="1" t="s">
@@ -2182,10 +2179,10 @@
       <c r="A44" s="2">
         <v>32</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>50</v>
       </c>
       <c r="M44" s="1" t="s">
@@ -2205,10 +2202,10 @@
       <c r="A45" s="2">
         <v>33</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>51</v>
       </c>
       <c r="M45" s="1" t="s">
@@ -2228,10 +2225,10 @@
       <c r="A46" s="2">
         <v>34</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2245,10 +2242,10 @@
       <c r="A47" s="2">
         <v>35</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2262,7 +2259,7 @@
       <c r="A48" s="2">
         <v>36</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2270,10 +2267,10 @@
       <c r="A49" s="2">
         <v>37</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2344,10 +2341,10 @@
       <c r="A50" s="2">
         <v>38</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>40</v>
       </c>
       <c r="H50" s="1" t="s">
@@ -2379,10 +2376,10 @@
       <c r="A51" s="2">
         <v>39</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>49</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -2414,10 +2411,10 @@
       <c r="A52" s="2">
         <v>40</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>50</v>
       </c>
       <c r="U52" s="1" t="s">
@@ -2437,10 +2434,10 @@
       <c r="A53" s="2">
         <v>41</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>51</v>
       </c>
       <c r="U53" s="1" t="s">
@@ -2460,10 +2457,10 @@
       <c r="A54" s="2">
         <v>42</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2495,10 +2492,10 @@
       <c r="A55" s="2">
         <v>43</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>53</v>
       </c>
       <c r="D55" s="1" t="s">

</xml_diff>